<commit_message>
PDF working on Azure
</commit_message>
<xml_diff>
--- a/HaverDevProject/ncr-template.xlsx
+++ b/HaverDevProject/ncr-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HaverNiagara\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HaverNiagara\V7\HaverProjectV2\HaverDevProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128EAED8-83B2-4542-A2E8-303BA15ED22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CD3C3D-CA3A-407C-83CF-19D778F9A196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29010" yWindow="630" windowWidth="18345" windowHeight="20475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NCR" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>If "Yes" indicate CAR #</t>
   </si>
   <si>
-    <t>If "Yes" indicate type &amp; expected date</t>
-  </si>
-  <si>
     <t>NCR Closed:</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
   </si>
   <si>
     <t>WIP (Production Order)</t>
-  </si>
-  <si>
-    <t>Quality Representative's Name:</t>
   </si>
   <si>
     <t>1/ Quality Representative</t>
@@ -245,9 +239,6 @@
     <t xml:space="preserve">Supplier Name                                            </t>
   </si>
   <si>
-    <t>Operations Manager:</t>
-  </si>
-  <si>
     <t>Does the drawing require updating</t>
   </si>
   <si>
@@ -330,12 +321,24 @@
   </si>
   <si>
     <t>5/ Reinspect</t>
+  </si>
+  <si>
+    <t>If "Yes" indicate expected date</t>
+  </si>
+  <si>
+    <t>Quality Representative:</t>
+  </si>
+  <si>
+    <t>Operations:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="17">
     <font>
       <sz val="11"/>
@@ -1016,7 +1019,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1295,14 +1298,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1325,6 +1320,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1406,6 +1419,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1468,98 +1489,86 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1914,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="AD33" activeCellId="2" sqref="T40:AA40 AD40:AH40 AD33:AH33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="AE44" activeCellId="6" sqref="AE15:AH15 AD26:AH26 AD33:AH33 AD32:AH32 AD40:AH40 AE43:AH43 AE44:AH44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="18" customHeight="1"/>
@@ -1937,192 +1946,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="9" customHeight="1">
-      <c r="A1" s="114" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="110" t="s">
+      <c r="A1" s="118" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="111"/>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="101"/>
-      <c r="AF1" s="102"/>
-      <c r="AG1" s="102"/>
-      <c r="AH1" s="103"/>
+      <c r="O1" s="115"/>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="115"/>
+      <c r="X1" s="115"/>
+      <c r="Y1" s="115"/>
+      <c r="Z1" s="115"/>
+      <c r="AA1" s="115"/>
+      <c r="AB1" s="115"/>
+      <c r="AC1" s="115"/>
+      <c r="AD1" s="115"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="106"/>
+      <c r="AG1" s="106"/>
+      <c r="AH1" s="107"/>
     </row>
     <row r="2" spans="1:34" ht="9.75" customHeight="1">
-      <c r="A2" s="116"/>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="113"/>
-      <c r="Z2" s="113"/>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="113"/>
-      <c r="AC2" s="113"/>
-      <c r="AD2" s="113"/>
-      <c r="AE2" s="104"/>
-      <c r="AF2" s="105"/>
-      <c r="AG2" s="105"/>
-      <c r="AH2" s="106"/>
+      <c r="A2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="117"/>
+      <c r="R2" s="117"/>
+      <c r="S2" s="117"/>
+      <c r="T2" s="117"/>
+      <c r="U2" s="117"/>
+      <c r="V2" s="117"/>
+      <c r="W2" s="117"/>
+      <c r="X2" s="117"/>
+      <c r="Y2" s="117"/>
+      <c r="Z2" s="117"/>
+      <c r="AA2" s="117"/>
+      <c r="AB2" s="117"/>
+      <c r="AC2" s="117"/>
+      <c r="AD2" s="117"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="109"/>
+      <c r="AG2" s="109"/>
+      <c r="AH2" s="110"/>
     </row>
     <row r="3" spans="1:34" ht="9" customHeight="1">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="122" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="124" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="119"/>
-      <c r="O3" s="119"/>
-      <c r="P3" s="119"/>
-      <c r="Q3" s="119"/>
-      <c r="R3" s="119"/>
-      <c r="S3" s="119"/>
-      <c r="T3" s="119"/>
-      <c r="U3" s="119"/>
-      <c r="V3" s="119"/>
-      <c r="W3" s="119"/>
-      <c r="X3" s="119"/>
-      <c r="Y3" s="120"/>
-      <c r="Z3" s="124" t="s">
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="123"/>
+      <c r="Q3" s="123"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="123"/>
+      <c r="U3" s="123"/>
+      <c r="V3" s="123"/>
+      <c r="W3" s="123"/>
+      <c r="X3" s="123"/>
+      <c r="Y3" s="124"/>
+      <c r="Z3" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="119"/>
-      <c r="AB3" s="119"/>
-      <c r="AC3" s="119"/>
-      <c r="AD3" s="120"/>
-      <c r="AE3" s="104"/>
-      <c r="AF3" s="105"/>
-      <c r="AG3" s="105"/>
-      <c r="AH3" s="106"/>
+      <c r="AA3" s="123"/>
+      <c r="AB3" s="123"/>
+      <c r="AC3" s="123"/>
+      <c r="AD3" s="124"/>
+      <c r="AE3" s="108"/>
+      <c r="AF3" s="109"/>
+      <c r="AG3" s="109"/>
+      <c r="AH3" s="110"/>
     </row>
     <row r="4" spans="1:34" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="125" t="s">
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="122"/>
-      <c r="H4" s="122"/>
-      <c r="I4" s="122"/>
-      <c r="J4" s="122"/>
-      <c r="K4" s="122"/>
-      <c r="L4" s="122"/>
-      <c r="M4" s="122"/>
-      <c r="N4" s="122"/>
-      <c r="O4" s="122"/>
-      <c r="P4" s="122"/>
-      <c r="Q4" s="122"/>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="122"/>
-      <c r="U4" s="122"/>
-      <c r="V4" s="122"/>
-      <c r="W4" s="122"/>
-      <c r="X4" s="122"/>
-      <c r="Y4" s="123"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="122"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="126"/>
+      <c r="K4" s="126"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="126"/>
+      <c r="N4" s="126"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="126"/>
+      <c r="Q4" s="126"/>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="126"/>
+      <c r="U4" s="126"/>
+      <c r="V4" s="126"/>
+      <c r="W4" s="126"/>
+      <c r="X4" s="126"/>
+      <c r="Y4" s="127"/>
+      <c r="Z4" s="129"/>
+      <c r="AA4" s="126"/>
       <c r="AB4" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC4" s="126"/>
-      <c r="AD4" s="127"/>
-      <c r="AE4" s="107"/>
-      <c r="AF4" s="108"/>
-      <c r="AG4" s="108"/>
-      <c r="AH4" s="109"/>
+        <v>32</v>
+      </c>
+      <c r="AC4" s="130"/>
+      <c r="AD4" s="131"/>
+      <c r="AE4" s="111"/>
+      <c r="AF4" s="112"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="113"/>
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1">
       <c r="A5" s="62" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="130" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" s="130"/>
-      <c r="O5" s="130"/>
-      <c r="P5" s="130"/>
-      <c r="Q5" s="130"/>
-      <c r="R5" s="130"/>
-      <c r="S5" s="130"/>
-      <c r="T5" s="130"/>
-      <c r="U5" s="130"/>
-      <c r="V5" s="130"/>
-      <c r="W5" s="131"/>
-      <c r="X5" s="128" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="136" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" s="136"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="136"/>
+      <c r="Q5" s="136"/>
+      <c r="R5" s="136"/>
+      <c r="S5" s="136"/>
+      <c r="T5" s="136"/>
+      <c r="U5" s="136"/>
+      <c r="V5" s="136"/>
+      <c r="W5" s="137"/>
+      <c r="X5" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="128"/>
-      <c r="Z5" s="128"/>
-      <c r="AA5" s="128"/>
-      <c r="AB5" s="128"/>
+      <c r="Y5" s="134"/>
+      <c r="Z5" s="134"/>
+      <c r="AA5" s="134"/>
+      <c r="AB5" s="134"/>
       <c r="AC5" s="67"/>
       <c r="AD5" s="67"/>
       <c r="AE5" s="67"/>
@@ -2135,7 +2144,7 @@
       <c r="B6" s="11"/>
       <c r="C6" s="17"/>
       <c r="D6" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2145,37 +2154,37 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="132"/>
-      <c r="P6" s="132"/>
-      <c r="Q6" s="132"/>
-      <c r="R6" s="132"/>
-      <c r="S6" s="132"/>
-      <c r="T6" s="132"/>
-      <c r="U6" s="132"/>
-      <c r="V6" s="132"/>
-      <c r="W6" s="132"/>
-      <c r="X6" s="141" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y6" s="141"/>
-      <c r="Z6" s="141"/>
-      <c r="AA6" s="141"/>
-      <c r="AB6" s="141"/>
-      <c r="AC6" s="133"/>
-      <c r="AD6" s="133"/>
-      <c r="AE6" s="133"/>
-      <c r="AF6" s="133"/>
-      <c r="AG6" s="133"/>
-      <c r="AH6" s="134"/>
+      <c r="M6" s="138"/>
+      <c r="N6" s="138"/>
+      <c r="O6" s="138"/>
+      <c r="P6" s="138"/>
+      <c r="Q6" s="138"/>
+      <c r="R6" s="138"/>
+      <c r="S6" s="138"/>
+      <c r="T6" s="138"/>
+      <c r="U6" s="138"/>
+      <c r="V6" s="138"/>
+      <c r="W6" s="138"/>
+      <c r="X6" s="147" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" s="147"/>
+      <c r="Z6" s="147"/>
+      <c r="AA6" s="147"/>
+      <c r="AB6" s="147"/>
+      <c r="AC6" s="139"/>
+      <c r="AD6" s="139"/>
+      <c r="AE6" s="139"/>
+      <c r="AF6" s="139"/>
+      <c r="AG6" s="139"/>
+      <c r="AH6" s="140"/>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1">
       <c r="A7" s="62"/>
       <c r="B7" s="7"/>
       <c r="C7" s="17"/>
       <c r="D7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="8"/>
       <c r="G7" s="9"/>
@@ -2184,59 +2193,59 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="129"/>
-      <c r="N7" s="129"/>
-      <c r="O7" s="129"/>
-      <c r="P7" s="129"/>
-      <c r="Q7" s="129"/>
-      <c r="R7" s="129"/>
-      <c r="S7" s="129"/>
-      <c r="T7" s="129"/>
-      <c r="U7" s="129"/>
-      <c r="V7" s="129"/>
-      <c r="W7" s="129"/>
-      <c r="X7" s="142" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y7" s="142"/>
-      <c r="Z7" s="142"/>
-      <c r="AA7" s="142"/>
-      <c r="AB7" s="142"/>
-      <c r="AC7" s="135"/>
-      <c r="AD7" s="135"/>
-      <c r="AE7" s="135"/>
-      <c r="AF7" s="135"/>
-      <c r="AG7" s="135"/>
-      <c r="AH7" s="136"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="135"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="135"/>
+      <c r="R7" s="135"/>
+      <c r="S7" s="135"/>
+      <c r="T7" s="135"/>
+      <c r="U7" s="135"/>
+      <c r="V7" s="135"/>
+      <c r="W7" s="135"/>
+      <c r="X7" s="148" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="148"/>
+      <c r="Z7" s="148"/>
+      <c r="AA7" s="148"/>
+      <c r="AB7" s="148"/>
+      <c r="AC7" s="141"/>
+      <c r="AD7" s="141"/>
+      <c r="AE7" s="141"/>
+      <c r="AF7" s="141"/>
+      <c r="AG7" s="141"/>
+      <c r="AH7" s="142"/>
     </row>
     <row r="8" spans="1:34" ht="15" customHeight="1">
       <c r="A8" s="62"/>
-      <c r="B8" s="139" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="139"/>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="139"/>
-      <c r="K8" s="139"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="139"/>
-      <c r="N8" s="139"/>
-      <c r="O8" s="139"/>
-      <c r="P8" s="139"/>
-      <c r="Q8" s="139"/>
-      <c r="R8" s="139"/>
-      <c r="S8" s="139"/>
-      <c r="T8" s="139"/>
-      <c r="U8" s="139"/>
-      <c r="V8" s="139"/>
-      <c r="W8" s="140"/>
+      <c r="B8" s="145" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
+      <c r="F8" s="145"/>
+      <c r="G8" s="145"/>
+      <c r="H8" s="145"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="145"/>
+      <c r="K8" s="145"/>
+      <c r="L8" s="145"/>
+      <c r="M8" s="145"/>
+      <c r="N8" s="145"/>
+      <c r="O8" s="145"/>
+      <c r="P8" s="145"/>
+      <c r="Q8" s="145"/>
+      <c r="R8" s="145"/>
+      <c r="S8" s="145"/>
+      <c r="T8" s="145"/>
+      <c r="U8" s="145"/>
+      <c r="V8" s="145"/>
+      <c r="W8" s="146"/>
       <c r="X8" s="74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y8" s="75"/>
       <c r="Z8" s="75"/>
@@ -2245,9 +2254,9 @@
       <c r="AC8" s="75"/>
       <c r="AD8" s="75"/>
       <c r="AE8" s="75"/>
-      <c r="AF8" s="143"/>
-      <c r="AG8" s="143"/>
-      <c r="AH8" s="144"/>
+      <c r="AF8" s="149"/>
+      <c r="AG8" s="149"/>
+      <c r="AH8" s="150"/>
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1">
       <c r="A9" s="62"/>
@@ -2283,14 +2292,14 @@
       <c r="AC9" s="75"/>
       <c r="AD9" s="75"/>
       <c r="AE9" s="75"/>
-      <c r="AF9" s="137"/>
-      <c r="AG9" s="137"/>
-      <c r="AH9" s="138"/>
+      <c r="AF9" s="143"/>
+      <c r="AG9" s="143"/>
+      <c r="AH9" s="144"/>
     </row>
     <row r="10" spans="1:34" ht="15" customHeight="1">
       <c r="A10" s="62"/>
       <c r="B10" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2399,66 +2408,66 @@
     </row>
     <row r="13" spans="1:34" ht="18" customHeight="1">
       <c r="A13" s="63"/>
-      <c r="B13" s="152" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="153"/>
-      <c r="D13" s="153"/>
-      <c r="E13" s="153"/>
-      <c r="F13" s="153"/>
-      <c r="G13" s="153"/>
-      <c r="H13" s="153"/>
-      <c r="I13" s="153"/>
-      <c r="J13" s="153"/>
-      <c r="K13" s="153"/>
-      <c r="L13" s="153"/>
-      <c r="M13" s="153"/>
-      <c r="N13" s="149" t="s">
-        <v>79</v>
-      </c>
-      <c r="O13" s="150"/>
-      <c r="P13" s="150"/>
-      <c r="Q13" s="150"/>
-      <c r="R13" s="150"/>
-      <c r="S13" s="150"/>
-      <c r="T13" s="150"/>
-      <c r="U13" s="150"/>
-      <c r="V13" s="150"/>
-      <c r="W13" s="150"/>
-      <c r="X13" s="150"/>
-      <c r="Y13" s="150"/>
-      <c r="Z13" s="150"/>
-      <c r="AA13" s="150"/>
-      <c r="AB13" s="150"/>
-      <c r="AC13" s="150"/>
-      <c r="AD13" s="150"/>
-      <c r="AE13" s="150"/>
-      <c r="AF13" s="150"/>
-      <c r="AG13" s="150"/>
-      <c r="AH13" s="151"/>
+      <c r="B13" s="156" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="157"/>
+      <c r="D13" s="157"/>
+      <c r="E13" s="157"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="157"/>
+      <c r="K13" s="157"/>
+      <c r="L13" s="157"/>
+      <c r="M13" s="157"/>
+      <c r="N13" s="153" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="154"/>
+      <c r="P13" s="154"/>
+      <c r="Q13" s="154"/>
+      <c r="R13" s="154"/>
+      <c r="S13" s="154"/>
+      <c r="T13" s="154"/>
+      <c r="U13" s="154"/>
+      <c r="V13" s="154"/>
+      <c r="W13" s="154"/>
+      <c r="X13" s="154"/>
+      <c r="Y13" s="154"/>
+      <c r="Z13" s="154"/>
+      <c r="AA13" s="154"/>
+      <c r="AB13" s="154"/>
+      <c r="AC13" s="154"/>
+      <c r="AD13" s="154"/>
+      <c r="AE13" s="154"/>
+      <c r="AF13" s="154"/>
+      <c r="AG13" s="154"/>
+      <c r="AH13" s="155"/>
     </row>
     <row r="14" spans="1:34" ht="15" customHeight="1">
       <c r="A14" s="62"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="154" t="s">
+      <c r="D14" s="151" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="105"/>
+      <c r="E14" s="109"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="154" t="s">
+      <c r="I14" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="105"/>
+      <c r="J14" s="109"/>
       <c r="T14" s="17"/>
-      <c r="U14" s="154" t="s">
+      <c r="U14" s="151" t="s">
         <v>13</v>
       </c>
-      <c r="V14" s="105"/>
+      <c r="V14" s="109"/>
       <c r="Y14" s="17"/>
-      <c r="Z14" s="154" t="s">
+      <c r="Z14" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="AA14" s="105"/>
+      <c r="AA14" s="109"/>
       <c r="AH14" s="24"/>
     </row>
     <row r="15" spans="1:34" ht="18" customHeight="1" thickBot="1">
@@ -2472,41 +2481,41 @@
       <c r="H15" s="26"/>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
-      <c r="K15" s="122" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="122"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="122"/>
-      <c r="O15" s="122"/>
-      <c r="P15" s="122"/>
-      <c r="Q15" s="122"/>
-      <c r="R15" s="122"/>
-      <c r="S15" s="122"/>
-      <c r="T15" s="122"/>
-      <c r="U15" s="155"/>
-      <c r="V15" s="155"/>
-      <c r="W15" s="155"/>
-      <c r="X15" s="155"/>
-      <c r="Y15" s="155"/>
-      <c r="Z15" s="155"/>
-      <c r="AA15" s="155"/>
-      <c r="AB15" s="122" t="s">
+      <c r="K15" s="126" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="126"/>
+      <c r="M15" s="126"/>
+      <c r="N15" s="126"/>
+      <c r="O15" s="126"/>
+      <c r="P15" s="126"/>
+      <c r="Q15" s="126"/>
+      <c r="R15" s="126"/>
+      <c r="S15" s="126"/>
+      <c r="T15" s="126"/>
+      <c r="U15" s="152"/>
+      <c r="V15" s="152"/>
+      <c r="W15" s="152"/>
+      <c r="X15" s="152"/>
+      <c r="Y15" s="152"/>
+      <c r="Z15" s="152"/>
+      <c r="AA15" s="152"/>
+      <c r="AB15" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="AC15" s="122"/>
-      <c r="AD15" s="122"/>
-      <c r="AE15" s="92"/>
-      <c r="AF15" s="92"/>
-      <c r="AG15" s="92"/>
-      <c r="AH15" s="93"/>
+      <c r="AC15" s="126"/>
+      <c r="AD15" s="126"/>
+      <c r="AE15" s="167"/>
+      <c r="AF15" s="167"/>
+      <c r="AG15" s="167"/>
+      <c r="AH15" s="168"/>
     </row>
     <row r="16" spans="1:34" ht="15" customHeight="1">
       <c r="A16" s="89" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -2584,16 +2593,16 @@
       <c r="O18" s="20"/>
       <c r="P18" s="20"/>
       <c r="Q18" s="17"/>
-      <c r="R18" s="154" t="s">
+      <c r="R18" s="151" t="s">
         <v>13</v>
       </c>
-      <c r="S18" s="105"/>
+      <c r="S18" s="109"/>
       <c r="T18" s="34"/>
       <c r="U18" s="17"/>
-      <c r="V18" s="154" t="s">
+      <c r="V18" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="W18" s="105"/>
+      <c r="W18" s="109"/>
       <c r="AA18" s="34"/>
       <c r="AH18" s="24"/>
     </row>
@@ -2675,7 +2684,7 @@
     </row>
     <row r="21" spans="1:34" ht="18" customHeight="1">
       <c r="A21" s="90"/>
-      <c r="B21" s="170"/>
+      <c r="B21" s="165"/>
       <c r="C21" s="65"/>
       <c r="D21" s="65"/>
       <c r="E21" s="65"/>
@@ -2711,7 +2720,7 @@
     </row>
     <row r="22" spans="1:34" ht="18" customHeight="1">
       <c r="A22" s="90"/>
-      <c r="B22" s="170"/>
+      <c r="B22" s="165"/>
       <c r="C22" s="65"/>
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
@@ -2747,32 +2756,32 @@
     </row>
     <row r="23" spans="1:34" ht="15" customHeight="1">
       <c r="A23" s="90"/>
-      <c r="B23" s="156" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="147"/>
-      <c r="D23" s="147"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="147"/>
-      <c r="G23" s="147"/>
-      <c r="H23" s="147"/>
-      <c r="I23" s="147"/>
-      <c r="J23" s="147"/>
-      <c r="K23" s="147"/>
-      <c r="L23" s="147"/>
-      <c r="M23" s="147"/>
+      <c r="B23" s="132" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="133"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="133"/>
+      <c r="H23" s="133"/>
+      <c r="I23" s="133"/>
+      <c r="J23" s="133"/>
+      <c r="K23" s="133"/>
+      <c r="L23" s="133"/>
+      <c r="M23" s="133"/>
       <c r="O23" s="17"/>
-      <c r="P23" s="105" t="s">
+      <c r="P23" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="Q23" s="105"/>
-      <c r="R23" s="105"/>
+      <c r="Q23" s="109"/>
+      <c r="R23" s="109"/>
       <c r="T23" s="17"/>
-      <c r="U23" s="105" t="s">
+      <c r="U23" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="V23" s="105"/>
-      <c r="W23" s="105"/>
+      <c r="V23" s="109"/>
+      <c r="W23" s="109"/>
       <c r="Z23" s="37"/>
       <c r="AA23" s="37"/>
       <c r="AB23" s="37"/>
@@ -2785,35 +2794,35 @@
     </row>
     <row r="24" spans="1:34" ht="15" customHeight="1">
       <c r="A24" s="90"/>
-      <c r="B24" s="156" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="147"/>
-      <c r="D24" s="147"/>
-      <c r="E24" s="147"/>
-      <c r="F24" s="147"/>
-      <c r="G24" s="147"/>
-      <c r="H24" s="147"/>
-      <c r="I24" s="147"/>
-      <c r="J24" s="148"/>
-      <c r="K24" s="148"/>
-      <c r="L24" s="148"/>
-      <c r="M24" s="148"/>
-      <c r="N24" s="147" t="s">
-        <v>57</v>
-      </c>
-      <c r="O24" s="147"/>
-      <c r="P24" s="147"/>
-      <c r="Q24" s="147"/>
-      <c r="R24" s="147"/>
+      <c r="B24" s="132" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="133"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
+      <c r="G24" s="133"/>
+      <c r="H24" s="133"/>
+      <c r="I24" s="133"/>
+      <c r="J24" s="159"/>
+      <c r="K24" s="159"/>
+      <c r="L24" s="159"/>
+      <c r="M24" s="159"/>
+      <c r="N24" s="133" t="s">
+        <v>54</v>
+      </c>
+      <c r="O24" s="133"/>
+      <c r="P24" s="133"/>
+      <c r="Q24" s="133"/>
+      <c r="R24" s="133"/>
       <c r="S24" s="37"/>
-      <c r="T24" s="148"/>
-      <c r="U24" s="148"/>
-      <c r="V24" s="148"/>
-      <c r="W24" s="148"/>
-      <c r="X24" s="148"/>
-      <c r="Y24" s="148"/>
-      <c r="Z24" s="148"/>
+      <c r="T24" s="159"/>
+      <c r="U24" s="159"/>
+      <c r="V24" s="159"/>
+      <c r="W24" s="159"/>
+      <c r="X24" s="159"/>
+      <c r="Y24" s="159"/>
+      <c r="Z24" s="159"/>
       <c r="AA24" s="37"/>
       <c r="AB24" s="37"/>
       <c r="AC24" s="37"/>
@@ -2825,35 +2834,35 @@
     </row>
     <row r="25" spans="1:34" ht="15" customHeight="1">
       <c r="A25" s="90"/>
-      <c r="B25" s="156" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="147"/>
-      <c r="D25" s="147"/>
-      <c r="E25" s="147"/>
-      <c r="F25" s="147"/>
-      <c r="G25" s="147"/>
-      <c r="H25" s="147"/>
-      <c r="I25" s="147"/>
-      <c r="J25" s="148"/>
-      <c r="K25" s="148"/>
-      <c r="L25" s="148"/>
-      <c r="M25" s="148"/>
-      <c r="N25" s="147" t="s">
-        <v>58</v>
-      </c>
-      <c r="O25" s="147"/>
-      <c r="P25" s="147"/>
-      <c r="Q25" s="147"/>
-      <c r="R25" s="147"/>
-      <c r="S25" s="147"/>
-      <c r="T25" s="148"/>
-      <c r="U25" s="148"/>
-      <c r="V25" s="148"/>
-      <c r="W25" s="148"/>
-      <c r="X25" s="148"/>
-      <c r="Y25" s="148"/>
-      <c r="Z25" s="148"/>
+      <c r="B25" s="132" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="133"/>
+      <c r="H25" s="133"/>
+      <c r="I25" s="133"/>
+      <c r="J25" s="159"/>
+      <c r="K25" s="159"/>
+      <c r="L25" s="159"/>
+      <c r="M25" s="159"/>
+      <c r="N25" s="133" t="s">
+        <v>55</v>
+      </c>
+      <c r="O25" s="133"/>
+      <c r="P25" s="133"/>
+      <c r="Q25" s="133"/>
+      <c r="R25" s="133"/>
+      <c r="S25" s="133"/>
+      <c r="T25" s="159"/>
+      <c r="U25" s="159"/>
+      <c r="V25" s="159"/>
+      <c r="W25" s="159"/>
+      <c r="X25" s="159"/>
+      <c r="Y25" s="159"/>
+      <c r="Z25" s="159"/>
       <c r="AA25" s="37"/>
       <c r="AB25" s="37"/>
       <c r="AC25" s="37"/>
@@ -2878,37 +2887,37 @@
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
       <c r="N26" s="73" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="O26" s="73"/>
       <c r="P26" s="73"/>
       <c r="Q26" s="73"/>
       <c r="R26" s="73"/>
       <c r="S26" s="73"/>
-      <c r="T26" s="159"/>
-      <c r="U26" s="159"/>
-      <c r="V26" s="159"/>
-      <c r="W26" s="159"/>
-      <c r="X26" s="159"/>
-      <c r="Y26" s="159"/>
-      <c r="Z26" s="159"/>
-      <c r="AA26" s="159"/>
+      <c r="T26" s="163"/>
+      <c r="U26" s="163"/>
+      <c r="V26" s="163"/>
+      <c r="W26" s="163"/>
+      <c r="X26" s="163"/>
+      <c r="Y26" s="163"/>
+      <c r="Z26" s="163"/>
+      <c r="AA26" s="163"/>
       <c r="AB26" s="26" t="s">
         <v>16</v>
       </c>
       <c r="AC26" s="26"/>
-      <c r="AD26" s="171"/>
-      <c r="AE26" s="159"/>
-      <c r="AF26" s="159"/>
-      <c r="AG26" s="159"/>
-      <c r="AH26" s="160"/>
+      <c r="AD26" s="169"/>
+      <c r="AE26" s="169"/>
+      <c r="AF26" s="169"/>
+      <c r="AG26" s="169"/>
+      <c r="AH26" s="170"/>
     </row>
     <row r="27" spans="1:34" ht="15" customHeight="1">
       <c r="A27" s="89" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
@@ -2924,7 +2933,7 @@
       <c r="N27" s="22"/>
       <c r="O27" s="41"/>
       <c r="P27" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q27" s="21"/>
       <c r="R27" s="21"/>
@@ -2949,19 +2958,19 @@
       <c r="A28" s="63"/>
       <c r="B28" s="17"/>
       <c r="C28" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="44"/>
       <c r="I28" s="44"/>
       <c r="K28" s="17"/>
       <c r="L28" s="44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q28" s="45"/>
       <c r="R28" s="45"/>
       <c r="S28" s="17"/>
       <c r="T28" s="79" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="U28" s="79"/>
       <c r="V28" s="79"/>
@@ -2976,7 +2985,7 @@
       <c r="AE28" s="79"/>
       <c r="AF28" s="79"/>
       <c r="AG28" s="79"/>
-      <c r="AH28" s="172"/>
+      <c r="AH28" s="166"/>
     </row>
     <row r="29" spans="1:34" ht="18" customHeight="1">
       <c r="A29" s="90"/>
@@ -3090,7 +3099,7 @@
     <row r="32" spans="1:34" ht="18" customHeight="1">
       <c r="A32" s="90"/>
       <c r="B32" s="79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" s="79"/>
       <c r="D32" s="79"/>
@@ -3109,7 +3118,7 @@
       </c>
       <c r="Q32" s="34"/>
       <c r="R32" s="48" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="W32" s="48"/>
       <c r="X32" s="48"/>
@@ -3118,11 +3127,11 @@
       <c r="AA32" s="48"/>
       <c r="AB32" s="48"/>
       <c r="AC32" s="48"/>
-      <c r="AD32" s="82"/>
-      <c r="AE32" s="82"/>
-      <c r="AF32" s="82"/>
-      <c r="AG32" s="82"/>
-      <c r="AH32" s="83"/>
+      <c r="AD32" s="171"/>
+      <c r="AE32" s="171"/>
+      <c r="AF32" s="171"/>
+      <c r="AG32" s="171"/>
+      <c r="AH32" s="172"/>
     </row>
     <row r="33" spans="1:34" ht="16.5" customHeight="1" thickBot="1">
       <c r="A33" s="91"/>
@@ -3139,7 +3148,7 @@
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
       <c r="N33" s="40" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="O33" s="27"/>
       <c r="P33" s="27"/>
@@ -3148,28 +3157,28 @@
       <c r="S33" s="27"/>
       <c r="T33" s="27"/>
       <c r="U33" s="29"/>
-      <c r="V33" s="155"/>
-      <c r="W33" s="155"/>
-      <c r="X33" s="155"/>
-      <c r="Y33" s="155"/>
-      <c r="Z33" s="155"/>
-      <c r="AA33" s="155"/>
+      <c r="V33" s="152"/>
+      <c r="W33" s="152"/>
+      <c r="X33" s="152"/>
+      <c r="Y33" s="152"/>
+      <c r="Z33" s="152"/>
+      <c r="AA33" s="152"/>
       <c r="AB33" s="26" t="s">
         <v>16</v>
       </c>
       <c r="AC33" s="26"/>
-      <c r="AD33" s="159"/>
-      <c r="AE33" s="159"/>
-      <c r="AF33" s="159"/>
-      <c r="AG33" s="159"/>
-      <c r="AH33" s="160"/>
+      <c r="AD33" s="169"/>
+      <c r="AE33" s="169"/>
+      <c r="AF33" s="169"/>
+      <c r="AG33" s="169"/>
+      <c r="AH33" s="170"/>
     </row>
     <row r="34" spans="1:34" ht="18" customHeight="1">
       <c r="A34" s="89" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
@@ -3182,7 +3191,7 @@
       <c r="K34" s="22"/>
       <c r="L34" s="41"/>
       <c r="M34" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N34" s="22"/>
       <c r="O34" s="51"/>
@@ -3199,7 +3208,7 @@
       <c r="Z34" s="21"/>
       <c r="AA34" s="41"/>
       <c r="AB34" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AC34" s="21"/>
       <c r="AD34" s="21"/>
@@ -3211,33 +3220,33 @@
     <row r="35" spans="1:34" ht="18" customHeight="1">
       <c r="A35" s="90"/>
       <c r="B35" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C35" s="44"/>
       <c r="D35" s="44"/>
-      <c r="H35" s="163"/>
-      <c r="I35" s="163"/>
-      <c r="J35" s="163"/>
-      <c r="K35" s="163"/>
-      <c r="L35" s="163"/>
-      <c r="M35" s="163"/>
-      <c r="N35" s="163"/>
+      <c r="H35" s="101"/>
+      <c r="I35" s="101"/>
+      <c r="J35" s="101"/>
+      <c r="K35" s="101"/>
+      <c r="L35" s="101"/>
+      <c r="M35" s="101"/>
+      <c r="N35" s="101"/>
       <c r="O35" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q35" s="45"/>
       <c r="R35" s="45"/>
       <c r="S35" s="34"/>
-      <c r="T35" s="163"/>
-      <c r="U35" s="163"/>
-      <c r="V35" s="163"/>
-      <c r="W35" s="163"/>
-      <c r="X35" s="163"/>
-      <c r="Y35" s="163"/>
-      <c r="Z35" s="163"/>
-      <c r="AA35" s="163"/>
-      <c r="AB35" s="163"/>
-      <c r="AC35" s="163"/>
+      <c r="T35" s="101"/>
+      <c r="U35" s="101"/>
+      <c r="V35" s="101"/>
+      <c r="W35" s="101"/>
+      <c r="X35" s="101"/>
+      <c r="Y35" s="101"/>
+      <c r="Z35" s="101"/>
+      <c r="AA35" s="101"/>
+      <c r="AB35" s="101"/>
+      <c r="AC35" s="101"/>
       <c r="AD35" s="46"/>
       <c r="AE35" s="46"/>
       <c r="AF35" s="46"/>
@@ -3247,33 +3256,33 @@
     <row r="36" spans="1:34" ht="18" customHeight="1">
       <c r="A36" s="90"/>
       <c r="B36" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C36" s="44"/>
       <c r="D36" s="44"/>
-      <c r="H36" s="163"/>
-      <c r="I36" s="163"/>
-      <c r="J36" s="163"/>
-      <c r="K36" s="163"/>
-      <c r="L36" s="163"/>
-      <c r="M36" s="163"/>
-      <c r="N36" s="163"/>
+      <c r="H36" s="101"/>
+      <c r="I36" s="101"/>
+      <c r="J36" s="101"/>
+      <c r="K36" s="101"/>
+      <c r="L36" s="101"/>
+      <c r="M36" s="101"/>
+      <c r="N36" s="101"/>
       <c r="O36" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q36" s="45"/>
       <c r="R36" s="45"/>
       <c r="S36" s="52"/>
-      <c r="T36" s="161"/>
-      <c r="U36" s="161"/>
-      <c r="V36" s="161"/>
-      <c r="W36" s="161"/>
-      <c r="X36" s="161"/>
-      <c r="Y36" s="161"/>
-      <c r="Z36" s="161"/>
-      <c r="AA36" s="161"/>
-      <c r="AB36" s="161"/>
-      <c r="AC36" s="161"/>
+      <c r="T36" s="164"/>
+      <c r="U36" s="164"/>
+      <c r="V36" s="164"/>
+      <c r="W36" s="164"/>
+      <c r="X36" s="164"/>
+      <c r="Y36" s="164"/>
+      <c r="Z36" s="164"/>
+      <c r="AA36" s="164"/>
+      <c r="AB36" s="164"/>
+      <c r="AC36" s="164"/>
       <c r="AD36" s="46"/>
       <c r="AE36" s="46"/>
       <c r="AF36" s="46"/>
@@ -3283,7 +3292,7 @@
     <row r="37" spans="1:34" ht="18" customHeight="1">
       <c r="A37" s="90"/>
       <c r="B37" s="79" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C37" s="79"/>
       <c r="D37" s="79"/>
@@ -3302,23 +3311,23 @@
         <v>14</v>
       </c>
       <c r="Q37" s="34"/>
-      <c r="W37" s="162"/>
-      <c r="X37" s="162"/>
-      <c r="Y37" s="162"/>
-      <c r="Z37" s="162"/>
-      <c r="AA37" s="162"/>
-      <c r="AB37" s="162"/>
-      <c r="AC37" s="162"/>
-      <c r="AD37" s="162"/>
-      <c r="AE37" s="167"/>
-      <c r="AF37" s="167"/>
-      <c r="AG37" s="167"/>
-      <c r="AH37" s="168"/>
+      <c r="W37" s="158"/>
+      <c r="X37" s="158"/>
+      <c r="Y37" s="158"/>
+      <c r="Z37" s="158"/>
+      <c r="AA37" s="158"/>
+      <c r="AB37" s="158"/>
+      <c r="AC37" s="158"/>
+      <c r="AD37" s="158"/>
+      <c r="AE37" s="160"/>
+      <c r="AF37" s="160"/>
+      <c r="AG37" s="160"/>
+      <c r="AH37" s="161"/>
     </row>
     <row r="38" spans="1:34" ht="18" customHeight="1">
       <c r="A38" s="90"/>
-      <c r="B38" s="169" t="s">
-        <v>70</v>
+      <c r="B38" s="162" t="s">
+        <v>67</v>
       </c>
       <c r="C38" s="79"/>
       <c r="D38" s="79"/>
@@ -3337,16 +3346,16 @@
         <v>14</v>
       </c>
       <c r="Q38" s="34"/>
-      <c r="T38" s="105" t="s">
-        <v>77</v>
-      </c>
-      <c r="U38" s="105"/>
-      <c r="V38" s="105"/>
-      <c r="W38" s="105"/>
-      <c r="X38" s="105"/>
-      <c r="Y38" s="105"/>
-      <c r="Z38" s="105"/>
-      <c r="AA38" s="105"/>
+      <c r="T38" s="109" t="s">
+        <v>74</v>
+      </c>
+      <c r="U38" s="109"/>
+      <c r="V38" s="109"/>
+      <c r="W38" s="109"/>
+      <c r="X38" s="109"/>
+      <c r="Y38" s="109"/>
+      <c r="Z38" s="109"/>
+      <c r="AA38" s="109"/>
       <c r="AB38" s="82"/>
       <c r="AC38" s="82"/>
       <c r="AD38" s="82"/>
@@ -3357,8 +3366,8 @@
     </row>
     <row r="39" spans="1:34" customFormat="1" ht="18" customHeight="1">
       <c r="A39" s="90"/>
-      <c r="B39" s="169" t="s">
-        <v>75</v>
+      <c r="B39" s="162" t="s">
+        <v>72</v>
       </c>
       <c r="C39" s="79"/>
       <c r="D39" s="79"/>
@@ -3394,37 +3403,37 @@
       <c r="L40" s="25"/>
       <c r="M40" s="25"/>
       <c r="N40" s="40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O40" s="27"/>
       <c r="P40" s="27"/>
       <c r="Q40" s="27"/>
       <c r="R40" s="27"/>
       <c r="S40" s="27"/>
-      <c r="T40" s="159"/>
-      <c r="U40" s="159"/>
-      <c r="V40" s="159"/>
-      <c r="W40" s="159"/>
-      <c r="X40" s="159"/>
-      <c r="Y40" s="159"/>
-      <c r="Z40" s="159"/>
-      <c r="AA40" s="159"/>
+      <c r="T40" s="163"/>
+      <c r="U40" s="163"/>
+      <c r="V40" s="163"/>
+      <c r="W40" s="163"/>
+      <c r="X40" s="163"/>
+      <c r="Y40" s="163"/>
+      <c r="Z40" s="163"/>
+      <c r="AA40" s="163"/>
       <c r="AB40" s="26" t="s">
         <v>16</v>
       </c>
       <c r="AC40" s="26"/>
-      <c r="AD40" s="159"/>
-      <c r="AE40" s="159"/>
-      <c r="AF40" s="159"/>
-      <c r="AG40" s="159"/>
-      <c r="AH40" s="160"/>
+      <c r="AD40" s="169"/>
+      <c r="AE40" s="169"/>
+      <c r="AF40" s="169"/>
+      <c r="AG40" s="169"/>
+      <c r="AH40" s="170"/>
     </row>
     <row r="41" spans="1:34" ht="15" customHeight="1">
       <c r="A41" s="89" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
@@ -3445,7 +3454,7 @@
       </c>
       <c r="P41" s="22"/>
       <c r="Q41" s="55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R41" s="42"/>
       <c r="S41" s="22"/>
@@ -3458,63 +3467,63 @@
       <c r="Z41" s="28"/>
       <c r="AA41" s="28"/>
       <c r="AB41" s="56"/>
-      <c r="AC41" s="165"/>
-      <c r="AD41" s="165"/>
-      <c r="AE41" s="165"/>
-      <c r="AF41" s="165"/>
-      <c r="AG41" s="165"/>
-      <c r="AH41" s="166"/>
+      <c r="AC41" s="103"/>
+      <c r="AD41" s="103"/>
+      <c r="AE41" s="103"/>
+      <c r="AF41" s="103"/>
+      <c r="AG41" s="103"/>
+      <c r="AH41" s="104"/>
     </row>
     <row r="42" spans="1:34" ht="18" customHeight="1">
       <c r="A42" s="90"/>
       <c r="B42" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C42" s="57"/>
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
-      <c r="F42" s="163"/>
-      <c r="G42" s="163"/>
-      <c r="H42" s="163"/>
-      <c r="I42" s="163"/>
-      <c r="J42" s="163"/>
-      <c r="K42" s="163"/>
-      <c r="L42" s="163"/>
-      <c r="M42" s="163"/>
-      <c r="N42" s="163"/>
-      <c r="O42" s="163"/>
-      <c r="P42" s="163"/>
-      <c r="Q42" s="163"/>
-      <c r="R42" s="163"/>
-      <c r="S42" s="163"/>
-      <c r="T42" s="163"/>
-      <c r="U42" s="163"/>
-      <c r="V42" s="163"/>
-      <c r="W42" s="163"/>
-      <c r="X42" s="163"/>
-      <c r="Y42" s="163"/>
-      <c r="Z42" s="163"/>
-      <c r="AA42" s="163"/>
-      <c r="AB42" s="163"/>
-      <c r="AC42" s="163"/>
-      <c r="AD42" s="163"/>
-      <c r="AE42" s="163"/>
-      <c r="AF42" s="163"/>
-      <c r="AG42" s="163"/>
-      <c r="AH42" s="164"/>
+      <c r="F42" s="101"/>
+      <c r="G42" s="101"/>
+      <c r="H42" s="101"/>
+      <c r="I42" s="101"/>
+      <c r="J42" s="101"/>
+      <c r="K42" s="101"/>
+      <c r="L42" s="101"/>
+      <c r="M42" s="101"/>
+      <c r="N42" s="101"/>
+      <c r="O42" s="101"/>
+      <c r="P42" s="101"/>
+      <c r="Q42" s="101"/>
+      <c r="R42" s="101"/>
+      <c r="S42" s="101"/>
+      <c r="T42" s="101"/>
+      <c r="U42" s="101"/>
+      <c r="V42" s="101"/>
+      <c r="W42" s="101"/>
+      <c r="X42" s="101"/>
+      <c r="Y42" s="101"/>
+      <c r="Z42" s="101"/>
+      <c r="AA42" s="101"/>
+      <c r="AB42" s="101"/>
+      <c r="AC42" s="101"/>
+      <c r="AD42" s="101"/>
+      <c r="AE42" s="101"/>
+      <c r="AF42" s="101"/>
+      <c r="AG42" s="101"/>
+      <c r="AH42" s="102"/>
     </row>
     <row r="43" spans="1:34" ht="18" customHeight="1">
       <c r="A43" s="90"/>
-      <c r="B43" s="145" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" s="146"/>
-      <c r="D43" s="146"/>
-      <c r="E43" s="146"/>
-      <c r="F43" s="146"/>
-      <c r="G43" s="146"/>
-      <c r="H43" s="146"/>
-      <c r="I43" s="146"/>
+      <c r="B43" s="99" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="100"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="100"/>
+      <c r="G43" s="100"/>
+      <c r="H43" s="100"/>
+      <c r="I43" s="100"/>
       <c r="J43" s="80"/>
       <c r="K43" s="80"/>
       <c r="L43" s="80"/>
@@ -3540,15 +3549,15 @@
       </c>
       <c r="AC43" s="88"/>
       <c r="AD43" s="88"/>
-      <c r="AE43" s="157"/>
-      <c r="AF43" s="157"/>
-      <c r="AG43" s="157"/>
-      <c r="AH43" s="158"/>
+      <c r="AE43" s="173"/>
+      <c r="AF43" s="173"/>
+      <c r="AG43" s="173"/>
+      <c r="AH43" s="174"/>
     </row>
     <row r="44" spans="1:34" ht="15.6" customHeight="1" thickBot="1">
       <c r="A44" s="91"/>
       <c r="B44" s="81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" s="73"/>
       <c r="D44" s="73"/>
@@ -3563,31 +3572,31 @@
       <c r="K44" s="25"/>
       <c r="L44" s="25"/>
       <c r="M44" s="25"/>
-      <c r="N44" s="94" t="s">
-        <v>50</v>
-      </c>
-      <c r="O44" s="94"/>
-      <c r="P44" s="94"/>
-      <c r="Q44" s="94"/>
-      <c r="R44" s="94"/>
-      <c r="S44" s="94"/>
-      <c r="T44" s="94"/>
-      <c r="U44" s="94"/>
-      <c r="V44" s="95"/>
-      <c r="W44" s="95"/>
-      <c r="X44" s="95"/>
-      <c r="Y44" s="95"/>
-      <c r="Z44" s="95"/>
-      <c r="AA44" s="95"/>
+      <c r="N44" s="92" t="s">
+        <v>48</v>
+      </c>
+      <c r="O44" s="92"/>
+      <c r="P44" s="92"/>
+      <c r="Q44" s="92"/>
+      <c r="R44" s="92"/>
+      <c r="S44" s="92"/>
+      <c r="T44" s="92"/>
+      <c r="U44" s="92"/>
+      <c r="V44" s="93"/>
+      <c r="W44" s="93"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
+      <c r="AA44" s="93"/>
       <c r="AB44" s="73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC44" s="73"/>
       <c r="AD44" s="73"/>
-      <c r="AE44" s="92"/>
-      <c r="AF44" s="92"/>
-      <c r="AG44" s="92"/>
-      <c r="AH44" s="93"/>
+      <c r="AE44" s="167"/>
+      <c r="AF44" s="167"/>
+      <c r="AG44" s="167"/>
+      <c r="AH44" s="168"/>
     </row>
     <row r="45" spans="1:34" ht="9.1999999999999993" customHeight="1">
       <c r="A45" s="59" t="s">
@@ -3636,46 +3645,46 @@
       <c r="AH45" s="72"/>
     </row>
     <row r="46" spans="1:34" ht="15" customHeight="1" thickBot="1">
-      <c r="A46" s="96" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="97"/>
-      <c r="C46" s="97"/>
-      <c r="D46" s="97"/>
-      <c r="E46" s="98"/>
-      <c r="F46" s="99">
+      <c r="A46" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="95"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="97">
         <v>41498</v>
       </c>
-      <c r="G46" s="99"/>
-      <c r="H46" s="99"/>
-      <c r="I46" s="99"/>
-      <c r="J46" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="K46" s="100"/>
-      <c r="L46" s="100"/>
-      <c r="M46" s="100"/>
-      <c r="N46" s="100"/>
-      <c r="O46" s="100"/>
-      <c r="P46" s="100"/>
-      <c r="Q46" s="100"/>
-      <c r="R46" s="100"/>
-      <c r="S46" s="100"/>
-      <c r="T46" s="100"/>
-      <c r="U46" s="100"/>
-      <c r="V46" s="100"/>
-      <c r="W46" s="100"/>
-      <c r="X46" s="100"/>
-      <c r="Y46" s="100"/>
-      <c r="Z46" s="100"/>
-      <c r="AA46" s="99">
+      <c r="G46" s="97"/>
+      <c r="H46" s="97"/>
+      <c r="I46" s="97"/>
+      <c r="J46" s="98" t="s">
+        <v>57</v>
+      </c>
+      <c r="K46" s="98"/>
+      <c r="L46" s="98"/>
+      <c r="M46" s="98"/>
+      <c r="N46" s="98"/>
+      <c r="O46" s="98"/>
+      <c r="P46" s="98"/>
+      <c r="Q46" s="98"/>
+      <c r="R46" s="98"/>
+      <c r="S46" s="98"/>
+      <c r="T46" s="98"/>
+      <c r="U46" s="98"/>
+      <c r="V46" s="98"/>
+      <c r="W46" s="98"/>
+      <c r="X46" s="98"/>
+      <c r="Y46" s="98"/>
+      <c r="Z46" s="98"/>
+      <c r="AA46" s="97">
         <v>45313</v>
       </c>
-      <c r="AB46" s="99"/>
-      <c r="AC46" s="99"/>
-      <c r="AD46" s="99"/>
+      <c r="AB46" s="97"/>
+      <c r="AC46" s="97"/>
+      <c r="AD46" s="97"/>
       <c r="AE46" s="84" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AF46" s="85"/>
       <c r="AG46" s="85"/>
@@ -3699,6 +3708,7 @@
     <mergeCell ref="T28:AH28"/>
     <mergeCell ref="N25:S25"/>
     <mergeCell ref="J25:M25"/>
+    <mergeCell ref="AD33:AH33"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="AE37:AH37"/>
     <mergeCell ref="B39:I39"/>
@@ -3711,24 +3721,20 @@
     <mergeCell ref="H35:N35"/>
     <mergeCell ref="T40:AA40"/>
     <mergeCell ref="AD40:AH40"/>
-    <mergeCell ref="AD33:AH33"/>
     <mergeCell ref="T36:AC36"/>
     <mergeCell ref="V33:AA33"/>
     <mergeCell ref="W37:AD37"/>
     <mergeCell ref="N24:R24"/>
     <mergeCell ref="T24:Z24"/>
     <mergeCell ref="T25:Z25"/>
+    <mergeCell ref="K15:T15"/>
+    <mergeCell ref="U15:AA15"/>
     <mergeCell ref="N13:AH13"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="Z14:AA14"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="U14:V14"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="AE15:AH15"/>
-    <mergeCell ref="K15:T15"/>
-    <mergeCell ref="U15:AA15"/>
     <mergeCell ref="B25:I25"/>
     <mergeCell ref="X5:AB5"/>
     <mergeCell ref="AB15:AD15"/>
@@ -3742,6 +3748,9 @@
     <mergeCell ref="X6:AB6"/>
     <mergeCell ref="X7:AB7"/>
     <mergeCell ref="AF8:AH8"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="AE15:AH15"/>
     <mergeCell ref="AE1:AH4"/>
     <mergeCell ref="N1:AD2"/>
     <mergeCell ref="A1:M2"/>

</xml_diff>